<commit_message>
add json reading function, place items into the map
</commit_message>
<xml_diff>
--- a/Treasure_coord_gold.xlsx
+++ b/Treasure_coord_gold.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>x</t>
   </si>
@@ -69,202 +69,13 @@
     <t>id</t>
   </si>
   <si>
-    <t>100M</t>
+    <t>amount1</t>
   </si>
   <si>
-    <t>1st amount</t>
+    <t>amount2</t>
   </si>
   <si>
-    <t>20M</t>
-  </si>
-  <si>
-    <t>5M</t>
-  </si>
-  <si>
-    <t>2nd amount</t>
-  </si>
-  <si>
-    <t>3rd amount</t>
-  </si>
-  <si>
-    <t>120M</t>
-  </si>
-  <si>
-    <t>30M</t>
-  </si>
-  <si>
-    <t>8M</t>
-  </si>
-  <si>
-    <t>24M</t>
-  </si>
-  <si>
-    <t>6M</t>
-  </si>
-  <si>
-    <t>150M</t>
-  </si>
-  <si>
-    <t>180M</t>
-  </si>
-  <si>
-    <t>36M</t>
-  </si>
-  <si>
-    <t>9M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30M </t>
-  </si>
-  <si>
-    <t>170M</t>
-  </si>
-  <si>
-    <t>34M</t>
-  </si>
-  <si>
-    <t>220M</t>
-  </si>
-  <si>
-    <t>44M</t>
-  </si>
-  <si>
-    <t>11M</t>
-  </si>
-  <si>
-    <t>200M</t>
-  </si>
-  <si>
-    <t>40M</t>
-  </si>
-  <si>
-    <t>10M</t>
-  </si>
-  <si>
-    <t>42M</t>
-  </si>
-  <si>
-    <t>250M</t>
-  </si>
-  <si>
-    <t>280M</t>
-  </si>
-  <si>
-    <t>50M</t>
-  </si>
-  <si>
-    <t>13M</t>
-  </si>
-  <si>
-    <t>56M</t>
-  </si>
-  <si>
-    <t>14M</t>
-  </si>
-  <si>
-    <t>270M</t>
-  </si>
-  <si>
-    <t>54M</t>
-  </si>
-  <si>
-    <t>300M</t>
-  </si>
-  <si>
-    <t>60M</t>
-  </si>
-  <si>
-    <t>15M</t>
-  </si>
-  <si>
-    <t>330M</t>
-  </si>
-  <si>
-    <t>66M</t>
-  </si>
-  <si>
-    <t>17M</t>
-  </si>
-  <si>
-    <t>360M</t>
-  </si>
-  <si>
-    <t>72M</t>
-  </si>
-  <si>
-    <t>18M</t>
-  </si>
-  <si>
-    <t>400M</t>
-  </si>
-  <si>
-    <t>80M</t>
-  </si>
-  <si>
-    <t>430M</t>
-  </si>
-  <si>
-    <t>450M</t>
-  </si>
-  <si>
-    <t>110M</t>
-  </si>
-  <si>
-    <t>35M</t>
-  </si>
-  <si>
-    <t>500M</t>
-  </si>
-  <si>
-    <t>550M</t>
-  </si>
-  <si>
-    <t>575M</t>
-  </si>
-  <si>
-    <t>600M</t>
-  </si>
-  <si>
-    <t>225M</t>
-  </si>
-  <si>
-    <t>65M</t>
-  </si>
-  <si>
-    <t>70M</t>
-  </si>
-  <si>
-    <t>650M</t>
-  </si>
-  <si>
-    <t>625M</t>
-  </si>
-  <si>
-    <t>700M</t>
-  </si>
-  <si>
-    <t>800M</t>
-  </si>
-  <si>
-    <t>900M</t>
-  </si>
-  <si>
-    <t>275M</t>
-  </si>
-  <si>
-    <t>75M</t>
-  </si>
-  <si>
-    <t>90M</t>
-  </si>
-  <si>
-    <t>95M</t>
-  </si>
-  <si>
-    <t>125M</t>
-  </si>
-  <si>
-    <t>175M</t>
+    <t>amount3</t>
   </si>
 </sst>
 </file>
@@ -598,7 +409,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,13 +434,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -645,14 +456,14 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,14 +479,14 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
+      <c r="E3">
+        <v>120</v>
+      </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -691,14 +502,14 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
+      <c r="E4">
+        <v>120</v>
+      </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -711,14 +522,14 @@
       <c r="C5">
         <v>3163</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
+      <c r="E5">
+        <v>150</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -731,14 +542,14 @@
       <c r="C6">
         <v>2855</v>
       </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
+      <c r="E6">
+        <v>180</v>
+      </c>
+      <c r="F6">
+        <v>36</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -751,14 +562,14 @@
       <c r="C7">
         <v>3021</v>
       </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
+      <c r="E7">
+        <v>150</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -771,14 +582,14 @@
       <c r="C8">
         <v>3380</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
+      <c r="E8">
+        <v>120</v>
+      </c>
+      <c r="F8">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -791,14 +602,14 @@
       <c r="C9">
         <v>3628</v>
       </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
+      <c r="E9">
+        <v>170</v>
+      </c>
+      <c r="F9">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -811,14 +622,14 @@
       <c r="C10">
         <v>3795</v>
       </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
+      <c r="E10">
+        <v>220</v>
+      </c>
+      <c r="F10">
+        <v>44</v>
+      </c>
+      <c r="G10">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -831,14 +642,14 @@
       <c r="C11">
         <v>3511</v>
       </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
+      <c r="E11">
+        <v>180</v>
+      </c>
+      <c r="F11">
+        <v>36</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -851,14 +662,14 @@
       <c r="C12">
         <v>3723</v>
       </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -871,14 +682,14 @@
       <c r="C13">
         <v>3870</v>
       </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" t="s">
-        <v>27</v>
+      <c r="E13">
+        <v>220</v>
+      </c>
+      <c r="F13">
+        <v>42</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -891,14 +702,14 @@
       <c r="C14">
         <v>3953</v>
       </c>
-      <c r="E14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" t="s">
-        <v>27</v>
+      <c r="E14">
+        <v>220</v>
+      </c>
+      <c r="F14">
+        <v>42</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -911,14 +722,14 @@
       <c r="C15">
         <v>4390</v>
       </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
+      <c r="E15">
+        <v>250</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -931,14 +742,14 @@
       <c r="C16">
         <v>4543</v>
       </c>
-      <c r="E16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>34</v>
+      <c r="E16">
+        <v>280</v>
+      </c>
+      <c r="F16">
+        <v>56</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -951,14 +762,14 @@
       <c r="C17">
         <v>4585</v>
       </c>
-      <c r="E17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" t="s">
-        <v>32</v>
+      <c r="E17">
+        <v>250</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -971,14 +782,14 @@
       <c r="C18">
         <v>4828</v>
       </c>
-      <c r="E18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" t="s">
-        <v>34</v>
+      <c r="E18">
+        <v>270</v>
+      </c>
+      <c r="F18">
+        <v>54</v>
+      </c>
+      <c r="G18">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -991,14 +802,14 @@
       <c r="C19">
         <v>5110</v>
       </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" t="s">
-        <v>34</v>
+      <c r="E19">
+        <v>270</v>
+      </c>
+      <c r="F19">
+        <v>54</v>
+      </c>
+      <c r="G19">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1011,14 +822,14 @@
       <c r="C20">
         <v>5240</v>
       </c>
-      <c r="E20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" t="s">
-        <v>39</v>
+      <c r="E20">
+        <v>300</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+      <c r="G20">
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1031,14 +842,14 @@
       <c r="C21">
         <v>4838</v>
       </c>
-      <c r="E21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" t="s">
-        <v>42</v>
+      <c r="E21">
+        <v>330</v>
+      </c>
+      <c r="F21">
+        <v>66</v>
+      </c>
+      <c r="G21">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1051,14 +862,14 @@
       <c r="C22">
         <v>5302</v>
       </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
+      <c r="E22">
+        <v>360</v>
+      </c>
+      <c r="F22">
+        <v>72</v>
+      </c>
+      <c r="G22">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1071,14 +882,14 @@
       <c r="C23">
         <v>5728</v>
       </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" t="s">
-        <v>42</v>
+      <c r="E23">
+        <v>330</v>
+      </c>
+      <c r="F23">
+        <v>66</v>
+      </c>
+      <c r="G23">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1091,14 +902,14 @@
       <c r="C24">
         <v>5950</v>
       </c>
-      <c r="E24" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" t="s">
-        <v>45</v>
+      <c r="E24">
+        <v>360</v>
+      </c>
+      <c r="F24">
+        <v>72</v>
+      </c>
+      <c r="G24">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1111,14 +922,14 @@
       <c r="C25">
         <v>6262</v>
       </c>
-      <c r="E25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" t="s">
-        <v>6</v>
+      <c r="E25">
+        <v>400</v>
+      </c>
+      <c r="F25">
+        <v>80</v>
+      </c>
+      <c r="G25">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1131,14 +942,14 @@
       <c r="C26">
         <v>6556</v>
       </c>
-      <c r="E26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>6</v>
+      <c r="E26">
+        <v>400</v>
+      </c>
+      <c r="F26">
+        <v>80</v>
+      </c>
+      <c r="G26">
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1151,14 +962,14 @@
       <c r="C27">
         <v>6760</v>
       </c>
-      <c r="E27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" t="s">
-        <v>11</v>
+      <c r="E27">
+        <v>430</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+      <c r="G27">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1171,14 +982,14 @@
       <c r="C28">
         <v>6963</v>
       </c>
-      <c r="E28" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" t="s">
-        <v>11</v>
+      <c r="E28">
+        <v>430</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+      <c r="G28">
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1191,14 +1002,14 @@
       <c r="C29">
         <v>6630</v>
       </c>
-      <c r="E29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" t="s">
-        <v>6</v>
+      <c r="E29">
+        <v>400</v>
+      </c>
+      <c r="F29">
+        <v>80</v>
+      </c>
+      <c r="G29">
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1211,14 +1022,14 @@
       <c r="C30">
         <v>6835</v>
       </c>
-      <c r="E30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" t="s">
-        <v>47</v>
-      </c>
-      <c r="G30" t="s">
-        <v>6</v>
+      <c r="E30">
+        <v>400</v>
+      </c>
+      <c r="F30">
+        <v>80</v>
+      </c>
+      <c r="G30">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1231,14 +1042,14 @@
       <c r="C31">
         <v>7033</v>
       </c>
-      <c r="E31" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" t="s">
-        <v>11</v>
+      <c r="E31">
+        <v>430</v>
+      </c>
+      <c r="F31">
+        <v>100</v>
+      </c>
+      <c r="G31">
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1251,14 +1062,14 @@
       <c r="C32">
         <v>7425</v>
       </c>
-      <c r="E32" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" t="s">
-        <v>51</v>
+      <c r="E32">
+        <v>450</v>
+      </c>
+      <c r="F32">
+        <v>110</v>
+      </c>
+      <c r="G32">
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1271,14 +1082,14 @@
       <c r="C33">
         <v>7570</v>
       </c>
-      <c r="E33" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" t="s">
-        <v>31</v>
+      <c r="E33">
+        <v>500</v>
+      </c>
+      <c r="F33">
+        <v>170</v>
+      </c>
+      <c r="G33">
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1291,14 +1102,14 @@
       <c r="C34">
         <v>7790</v>
       </c>
-      <c r="E34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" t="s">
-        <v>31</v>
+      <c r="E34">
+        <v>500</v>
+      </c>
+      <c r="F34">
+        <v>170</v>
+      </c>
+      <c r="G34">
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1311,14 +1122,14 @@
       <c r="C35">
         <v>7817</v>
       </c>
-      <c r="E35" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" t="s">
-        <v>31</v>
+      <c r="E35">
+        <v>500</v>
+      </c>
+      <c r="F35">
+        <v>170</v>
+      </c>
+      <c r="G35">
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1331,14 +1142,14 @@
       <c r="C36">
         <v>8125</v>
       </c>
-      <c r="E36" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" t="s">
-        <v>38</v>
+      <c r="E36">
+        <v>550</v>
+      </c>
+      <c r="F36">
+        <v>200</v>
+      </c>
+      <c r="G36">
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1351,14 +1162,14 @@
       <c r="C37">
         <v>8155</v>
       </c>
-      <c r="E37" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" t="s">
-        <v>38</v>
+      <c r="E37">
+        <v>550</v>
+      </c>
+      <c r="F37">
+        <v>200</v>
+      </c>
+      <c r="G37">
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1371,14 +1182,14 @@
       <c r="C38">
         <v>8411</v>
       </c>
-      <c r="E38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" t="s">
-        <v>56</v>
-      </c>
-      <c r="G38" t="s">
-        <v>57</v>
+      <c r="E38">
+        <v>575</v>
+      </c>
+      <c r="F38">
+        <v>225</v>
+      </c>
+      <c r="G38">
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1391,14 +1202,14 @@
       <c r="C39">
         <v>8365</v>
       </c>
-      <c r="E39" t="s">
-        <v>54</v>
-      </c>
-      <c r="F39" t="s">
-        <v>56</v>
-      </c>
-      <c r="G39" t="s">
-        <v>57</v>
+      <c r="E39">
+        <v>575</v>
+      </c>
+      <c r="F39">
+        <v>225</v>
+      </c>
+      <c r="G39">
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1411,14 +1222,14 @@
       <c r="C40">
         <v>8592</v>
       </c>
-      <c r="E40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" t="s">
-        <v>29</v>
-      </c>
-      <c r="G40" t="s">
-        <v>58</v>
+      <c r="E40">
+        <v>600</v>
+      </c>
+      <c r="F40">
+        <v>250</v>
+      </c>
+      <c r="G40">
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1431,14 +1242,14 @@
       <c r="C41">
         <v>8828</v>
       </c>
-      <c r="E41" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" t="s">
-        <v>64</v>
-      </c>
-      <c r="G41" t="s">
-        <v>66</v>
+      <c r="E41">
+        <v>650</v>
+      </c>
+      <c r="F41">
+        <v>275</v>
+      </c>
+      <c r="G41">
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1451,14 +1262,14 @@
       <c r="C42">
         <v>9200</v>
       </c>
-      <c r="E42" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" t="s">
-        <v>29</v>
-      </c>
-      <c r="G42" t="s">
-        <v>47</v>
+      <c r="E42">
+        <v>625</v>
+      </c>
+      <c r="F42">
+        <v>250</v>
+      </c>
+      <c r="G42">
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,14 +1282,14 @@
       <c r="C43">
         <v>8846</v>
       </c>
-      <c r="E43" t="s">
-        <v>60</v>
-      </c>
-      <c r="F43" t="s">
-        <v>29</v>
-      </c>
-      <c r="G43" t="s">
-        <v>47</v>
+      <c r="E43">
+        <v>625</v>
+      </c>
+      <c r="F43">
+        <v>250</v>
+      </c>
+      <c r="G43">
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1491,14 +1302,14 @@
       <c r="C44">
         <v>9120</v>
       </c>
-      <c r="E44" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G44" t="s">
-        <v>67</v>
+      <c r="E44">
+        <v>650</v>
+      </c>
+      <c r="F44">
+        <v>275</v>
+      </c>
+      <c r="G44">
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1511,14 +1322,14 @@
       <c r="C45">
         <v>8920</v>
       </c>
-      <c r="E45" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" t="s">
-        <v>67</v>
+      <c r="E45">
+        <v>650</v>
+      </c>
+      <c r="F45">
+        <v>275</v>
+      </c>
+      <c r="G45">
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1531,14 +1342,14 @@
       <c r="C46">
         <v>9286</v>
       </c>
-      <c r="E46" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46" t="s">
-        <v>29</v>
-      </c>
-      <c r="G46" t="s">
-        <v>65</v>
+      <c r="E46">
+        <v>600</v>
+      </c>
+      <c r="F46">
+        <v>250</v>
+      </c>
+      <c r="G46">
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1551,14 +1362,14 @@
       <c r="C47">
         <v>9569</v>
       </c>
-      <c r="E47" t="s">
-        <v>61</v>
-      </c>
-      <c r="F47" t="s">
-        <v>37</v>
-      </c>
-      <c r="G47" t="s">
-        <v>68</v>
+      <c r="E47">
+        <v>700</v>
+      </c>
+      <c r="F47">
+        <v>300</v>
+      </c>
+      <c r="G47">
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1571,14 +1382,14 @@
       <c r="C48">
         <v>9823</v>
       </c>
-      <c r="E48" t="s">
-        <v>62</v>
-      </c>
-      <c r="F48" t="s">
-        <v>46</v>
-      </c>
-      <c r="G48" t="s">
-        <v>69</v>
+      <c r="E48">
+        <v>800</v>
+      </c>
+      <c r="F48">
+        <v>400</v>
+      </c>
+      <c r="G48">
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1591,14 +1402,14 @@
       <c r="C49">
         <v>10010</v>
       </c>
-      <c r="E49" t="s">
-        <v>63</v>
-      </c>
-      <c r="F49" t="s">
-        <v>49</v>
-      </c>
-      <c r="G49" t="s">
-        <v>25</v>
+      <c r="E49">
+        <v>900</v>
+      </c>
+      <c r="F49">
+        <v>450</v>
+      </c>
+      <c r="G49">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pickup icons and fuel
</commit_message>
<xml_diff>
--- a/Treasure_coord_gold.xlsx
+++ b/Treasure_coord_gold.xlsx
@@ -45,8 +45,8 @@
           </rPr>
           <t xml:space="preserve">
 1. coin
-2. small chest
-3. large chest</t>
+2. chest
+3. fuel</t>
         </r>
       </text>
     </comment>
@@ -409,7 +409,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,16 +500,16 @@
         <v>2863</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>120</v>
+        <v>500</v>
       </c>
       <c r="F4">
-        <v>24</v>
+        <v>500</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -522,6 +522,9 @@
       <c r="C5">
         <v>3163</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="E5">
         <v>150</v>
       </c>
@@ -542,6 +545,9 @@
       <c r="C6">
         <v>2855</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6">
         <v>180</v>
       </c>
@@ -562,6 +568,9 @@
       <c r="C7">
         <v>3021</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="E7">
         <v>150</v>
       </c>
@@ -582,14 +591,17 @@
       <c r="C8">
         <v>3380</v>
       </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
       <c r="E8">
-        <v>120</v>
+        <v>500</v>
       </c>
       <c r="F8">
-        <v>24</v>
+        <v>500</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -602,6 +614,9 @@
       <c r="C9">
         <v>3628</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9">
         <v>170</v>
       </c>
@@ -622,6 +637,9 @@
       <c r="C10">
         <v>3795</v>
       </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
       <c r="E10">
         <v>220</v>
       </c>
@@ -642,6 +660,9 @@
       <c r="C11">
         <v>3511</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="E11">
         <v>180</v>
       </c>
@@ -662,6 +683,9 @@
       <c r="C12">
         <v>3723</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="E12">
         <v>200</v>
       </c>
@@ -682,6 +706,9 @@
       <c r="C13">
         <v>3870</v>
       </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="E13">
         <v>220</v>
       </c>
@@ -702,6 +729,9 @@
       <c r="C14">
         <v>3953</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="E14">
         <v>220</v>
       </c>
@@ -722,14 +752,17 @@
       <c r="C15">
         <v>4390</v>
       </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
       <c r="E15">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="F15">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="G15">
-        <v>13</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -742,6 +775,9 @@
       <c r="C16">
         <v>4543</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="E16">
         <v>280</v>
       </c>
@@ -762,6 +798,9 @@
       <c r="C17">
         <v>4585</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="E17">
         <v>250</v>
       </c>
@@ -782,6 +821,9 @@
       <c r="C18">
         <v>4828</v>
       </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
       <c r="E18">
         <v>270</v>
       </c>
@@ -802,6 +844,9 @@
       <c r="C19">
         <v>5110</v>
       </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
       <c r="E19">
         <v>270</v>
       </c>
@@ -822,6 +867,9 @@
       <c r="C20">
         <v>5240</v>
       </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
       <c r="E20">
         <v>300</v>
       </c>
@@ -842,6 +890,9 @@
       <c r="C21">
         <v>4838</v>
       </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
       <c r="E21">
         <v>330</v>
       </c>
@@ -862,6 +913,9 @@
       <c r="C22">
         <v>5302</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
       <c r="E22">
         <v>360</v>
       </c>
@@ -882,6 +936,9 @@
       <c r="C23">
         <v>5728</v>
       </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
       <c r="E23">
         <v>330</v>
       </c>
@@ -902,14 +959,17 @@
       <c r="C24">
         <v>5950</v>
       </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
       <c r="E24">
-        <v>360</v>
+        <v>500</v>
       </c>
       <c r="F24">
-        <v>72</v>
+        <v>500</v>
       </c>
       <c r="G24">
-        <v>18</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -922,14 +982,17 @@
       <c r="C25">
         <v>6262</v>
       </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
       <c r="E25">
-        <v>400</v>
+        <v>430</v>
       </c>
       <c r="F25">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G25">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -942,6 +1005,9 @@
       <c r="C26">
         <v>6556</v>
       </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
       <c r="E26">
         <v>400</v>
       </c>
@@ -962,14 +1028,17 @@
       <c r="C27">
         <v>6760</v>
       </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
       <c r="E27">
-        <v>430</v>
+        <v>500</v>
       </c>
       <c r="F27">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="G27">
-        <v>30</v>
+        <v>500</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -982,6 +1051,9 @@
       <c r="C28">
         <v>6963</v>
       </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
       <c r="E28">
         <v>430</v>
       </c>
@@ -1002,6 +1074,9 @@
       <c r="C29">
         <v>6630</v>
       </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
       <c r="E29">
         <v>400</v>
       </c>
@@ -1022,6 +1097,9 @@
       <c r="C30">
         <v>6835</v>
       </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
       <c r="E30">
         <v>400</v>
       </c>
@@ -1042,6 +1120,9 @@
       <c r="C31">
         <v>7033</v>
       </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
       <c r="E31">
         <v>430</v>
       </c>
@@ -1062,6 +1143,9 @@
       <c r="C32">
         <v>7425</v>
       </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
       <c r="E32">
         <v>450</v>
       </c>
@@ -1082,14 +1166,17 @@
       <c r="C33">
         <v>7570</v>
       </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
       <c r="E33">
         <v>500</v>
       </c>
       <c r="F33">
-        <v>170</v>
+        <v>500</v>
       </c>
       <c r="G33">
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1102,6 +1189,9 @@
       <c r="C34">
         <v>7790</v>
       </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
       <c r="E34">
         <v>500</v>
       </c>
@@ -1122,6 +1212,9 @@
       <c r="C35">
         <v>7817</v>
       </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
       <c r="E35">
         <v>500</v>
       </c>
@@ -1142,6 +1235,9 @@
       <c r="C36">
         <v>8125</v>
       </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
       <c r="E36">
         <v>550</v>
       </c>
@@ -1162,6 +1258,9 @@
       <c r="C37">
         <v>8155</v>
       </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
       <c r="E37">
         <v>550</v>
       </c>
@@ -1182,6 +1281,9 @@
       <c r="C38">
         <v>8411</v>
       </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
       <c r="E38">
         <v>575</v>
       </c>
@@ -1202,6 +1304,9 @@
       <c r="C39">
         <v>8365</v>
       </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
       <c r="E39">
         <v>575</v>
       </c>
@@ -1222,6 +1327,9 @@
       <c r="C40">
         <v>8592</v>
       </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
       <c r="E40">
         <v>600</v>
       </c>
@@ -1242,6 +1350,9 @@
       <c r="C41">
         <v>8828</v>
       </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
       <c r="E41">
         <v>650</v>
       </c>
@@ -1262,6 +1373,9 @@
       <c r="C42">
         <v>9200</v>
       </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
       <c r="E42">
         <v>625</v>
       </c>
@@ -1282,14 +1396,17 @@
       <c r="C43">
         <v>8846</v>
       </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
       <c r="E43">
-        <v>625</v>
+        <v>500</v>
       </c>
       <c r="F43">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="G43">
-        <v>80</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1302,6 +1419,9 @@
       <c r="C44">
         <v>9120</v>
       </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
       <c r="E44">
         <v>650</v>
       </c>
@@ -1322,6 +1442,9 @@
       <c r="C45">
         <v>8920</v>
       </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
       <c r="E45">
         <v>650</v>
       </c>
@@ -1342,6 +1465,9 @@
       <c r="C46">
         <v>9286</v>
       </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
       <c r="E46">
         <v>600</v>
       </c>
@@ -1362,6 +1488,9 @@
       <c r="C47">
         <v>9569</v>
       </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
       <c r="E47">
         <v>700</v>
       </c>
@@ -1382,6 +1511,9 @@
       <c r="C48">
         <v>9823</v>
       </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
       <c r="E48">
         <v>800</v>
       </c>
@@ -1402,14 +1534,17 @@
       <c r="C49">
         <v>10010</v>
       </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
       <c r="E49">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="F49">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="G49">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>